<commit_message>
feat(generate): api prefix 可配置
</commit_message>
<xml_diff>
--- a/sql/table.xlsx
+++ b/sql/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>表名</t>
   </si>
@@ -40,37 +40,43 @@
     <t>com.hyperchain</t>
   </si>
   <si>
+    <t>请求前缀</t>
+  </si>
+  <si>
+    <t>/platform/feedback</t>
+  </si>
+  <si>
     <t>目录映射</t>
   </si>
   <si>
     <t>controller</t>
   </si>
   <si>
-    <t>platform/controller/feedback</t>
+    <t>platform/feedback/controller</t>
   </si>
   <si>
     <t>vo</t>
   </si>
   <si>
-    <t>platform/controller/feedback/vo</t>
+    <t>platform/feedback/controller/vo</t>
   </si>
   <si>
     <t>service</t>
   </si>
   <si>
-    <t>platform/service</t>
+    <t>platform/feedback/service</t>
   </si>
   <si>
     <t>domain</t>
   </si>
   <si>
-    <t>platform/domain</t>
+    <t>platform/feedback/domain</t>
   </si>
   <si>
     <t>convert</t>
   </si>
   <si>
-    <t>platform/convert</t>
+    <t>platform/feedback/convert</t>
   </si>
   <si>
     <t>Name</t>
@@ -1162,7 +1168,7 @@
   <dimension ref="A1:Z40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1214,9 +1220,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="7" customFormat="1" spans="1:26">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1246,18 +1260,18 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:26">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1286,26 +1300,26 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:26">
@@ -1338,63 +1352,63 @@
     </row>
     <row r="20" s="2" customFormat="1" spans="1:16">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="1:26">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1436,13 +1450,13 @@
     </row>
     <row r="22" customFormat="1" spans="1:16">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>24</v>
@@ -1462,13 +1476,13 @@
     </row>
     <row r="23" customFormat="1" spans="1:26">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1504,13 +1518,13 @@
     </row>
     <row r="24" customFormat="1" spans="1:16">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1527,13 +1541,13 @@
     </row>
     <row r="25" customFormat="1" spans="1:26">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1565,13 +1579,13 @@
     </row>
     <row r="26" customFormat="1" spans="1:16">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O26" t="b">
         <v>1</v>
@@ -1582,17 +1596,17 @@
     </row>
     <row r="27" customFormat="1" spans="1:26">
       <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1620,27 +1634,27 @@
     </row>
     <row r="28" customFormat="1" spans="1:5">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" t="s">
         <v>56</v>
-      </c>
-      <c r="E28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:26">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>

</xml_diff>